<commit_message>
Increased silent time before preview
</commit_message>
<xml_diff>
--- a/inputs/conversion_data.xlsx
+++ b/inputs/conversion_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TaikoNS2Converter\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B89137-CA7E-49DA-AAF3-ECB9A0F3D11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870713DD-28D7-4273-B5BD-75B51C8D8792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="25981" windowHeight="13977" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>SONG_ID</t>
   </si>
@@ -79,13 +79,7 @@
     <t>GENRE</t>
   </si>
   <si>
-    <t>clscam</t>
-  </si>
-  <si>
-    <t>crtesc</t>
-  </si>
-  <si>
-    <t>fmod</t>
+    <t>batimt</t>
   </si>
 </sst>
 </file>
@@ -934,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A89AA7-337B-4B0E-947D-11A48156C344}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.1" x14ac:dyDescent="0.3"/>
@@ -1010,70 +1004,6 @@
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1">
-        <v>6</v>
-      </c>
-      <c r="I4" s="1">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix balloon count bug
</commit_message>
<xml_diff>
--- a/inputs/conversion_data.xlsx
+++ b/inputs/conversion_data.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TaikoNS2Converter\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5706C2-7575-4854-993B-08D07D806AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB16AD03-31B6-4B2F-980E-96D464644A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="25981" windowHeight="13977" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>SONG_ID</t>
   </si>
@@ -79,19 +90,22 @@
     <t>GENRE</t>
   </si>
   <si>
-    <t>badguy</t>
-  </si>
-  <si>
-    <t>mgadh</t>
-  </si>
-  <si>
-    <t>teknow</t>
-  </si>
-  <si>
-    <t>cpyoak</t>
-  </si>
-  <si>
-    <t>dobakb</t>
+    <t>sw2op</t>
+  </si>
+  <si>
+    <t>まいにちがドンダフル</t>
+  </si>
+  <si>
+    <t>「太鼓の達人 ドンダフルフェスティバル」テーマソング</t>
+  </si>
+  <si>
+    <t>夢うつつカタルシス</t>
+  </si>
+  <si>
+    <t>yumeut</t>
+  </si>
+  <si>
+    <t>大木奏弥(BNSI) feat. 愛原圭織</t>
   </si>
 </sst>
 </file>
@@ -940,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A89AA7-337B-4B0E-947D-11A48156C344}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.1" x14ac:dyDescent="0.3"/>
@@ -1016,25 +1030,52 @@
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed ways of adding preview sound
</commit_message>
<xml_diff>
--- a/inputs/conversion_data.xlsx
+++ b/inputs/conversion_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TaikoNS2Converter\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB16AD03-31B6-4B2F-980E-96D464644A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF031AC-E306-4CF8-B669-538170B21D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-101" yWindow="-101" windowWidth="25981" windowHeight="13977" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>SONG_ID</t>
   </si>
@@ -90,22 +90,19 @@
     <t>GENRE</t>
   </si>
   <si>
-    <t>sw2op</t>
-  </si>
-  <si>
-    <t>まいにちがドンダフル</t>
-  </si>
-  <si>
-    <t>「太鼓の達人 ドンダフルフェスティバル」テーマソング</t>
-  </si>
-  <si>
-    <t>夢うつつカタルシス</t>
-  </si>
-  <si>
-    <t>yumeut</t>
-  </si>
-  <si>
-    <t>大木奏弥(BNSI) feat. 愛原圭織</t>
+    <t>tontwi</t>
+  </si>
+  <si>
+    <t>TAIKO-TONGUE-TWISTER</t>
+  </si>
+  <si>
+    <t>Cory Tarrow(BNSI) feat. M.Polak, Avigail D., L.Munoz and Bryan D.</t>
+  </si>
+  <si>
+    <t>ohdsub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Subtitle</t>
   </si>
 </sst>
 </file>
@@ -957,7 +954,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.1" x14ac:dyDescent="0.3"/>
@@ -1043,39 +1040,48 @@
         <v>8</v>
       </c>
       <c r="G2" s="1">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1">
         <v>5</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1">
+      <c r="F3" s="1">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1">
-        <v>6</v>
-      </c>
       <c r="H3" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I3" s="1">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3560</v>
+      </c>
+      <c r="L3" s="1">
+        <v>5650</v>
+      </c>
+      <c r="M3" s="1">
+        <v>8370</v>
+      </c>
+      <c r="N3" s="1">
+        <v>12780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added direct datatable injection
</commit_message>
<xml_diff>
--- a/inputs/conversion_data.xlsx
+++ b/inputs/conversion_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TaikoNS2Converter\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\TaikoNS2Converter\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C70F2F-0CCC-40F9-9FFF-23E3D26A50FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB6490C-208B-450E-8FB4-EBA88672190D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13252" yWindow="3736" windowWidth="10322" windowHeight="8690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11168" yWindow="4531" windowWidth="10321" windowHeight="8691" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>SONG_ID</t>
   </si>
@@ -90,22 +90,7 @@
     <t>GENRE</t>
   </si>
   <si>
-    <t>tontwi</t>
-  </si>
-  <si>
-    <t>ohdsub</t>
-  </si>
-  <si>
-    <t>mksskn</t>
-  </si>
-  <si>
-    <t>sw2op</t>
-  </si>
-  <si>
-    <t>vfgbs</t>
-  </si>
-  <si>
-    <t>ohdmi2</t>
+    <t>dogma1</t>
   </si>
 </sst>
 </file>
@@ -954,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A89AA7-337B-4B0E-947D-11A48156C344}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.1" x14ac:dyDescent="0.3"/>
@@ -1031,31 +1016,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Adapt to new ver
</commit_message>
<xml_diff>
--- a/inputs/conversion_data.xlsx
+++ b/inputs/conversion_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\TaikoNS2Converter\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB6490C-208B-450E-8FB4-EBA88672190D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822271DD-ABD4-4A9D-8C75-1127A0ED379C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11168" yWindow="4531" windowWidth="10321" windowHeight="8691" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-101" yWindow="-101" windowWidth="25981" windowHeight="13977" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>SONG_ID</t>
   </si>
@@ -90,7 +90,13 @@
     <t>GENRE</t>
   </si>
   <si>
-    <t>dogma1</t>
+    <t>anochu</t>
+  </si>
+  <si>
+    <t>ちゅ、多様性。</t>
+  </si>
+  <si>
+    <t>TVアニメ「チェンソーマン」エンディング・テーマ</t>
   </si>
 </sst>
 </file>
@@ -942,7 +948,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.1" x14ac:dyDescent="0.3"/>
@@ -1015,6 +1021,27 @@
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed available uniqueid to start from 1
</commit_message>
<xml_diff>
--- a/inputs/conversion_data.xlsx
+++ b/inputs/conversion_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\TaikoNS2Converter\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822271DD-ABD4-4A9D-8C75-1127A0ED379C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CC679D-84C2-4D94-90F1-6CE0FCAAA827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-101" yWindow="-101" windowWidth="25981" windowHeight="13977" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9900" yWindow="6165" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>SONG_ID</t>
   </si>
@@ -90,13 +90,10 @@
     <t>GENRE</t>
   </si>
   <si>
-    <t>anochu</t>
-  </si>
-  <si>
-    <t>ちゅ、多様性。</t>
-  </si>
-  <si>
-    <t>TVアニメ「チェンソーマン」エンディング・テーマ</t>
+    <t>pkmdkm</t>
+  </si>
+  <si>
+    <t>gdmsen</t>
   </si>
 </sst>
 </file>
@@ -945,20 +942,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A89AA7-337B-4B0E-947D-11A48156C344}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="11.6328125" style="1"/>
-    <col min="5" max="5" width="11.6328125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.6328125" style="1"/>
+    <col min="1" max="4" width="11.5703125" style="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1017,30 +1014,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>